<commit_message>
[what] add cyrptographic hashing function, add decrypt and compare function for homomorphic encrypted results, refactor the excel operations into a saperate file, update __init__.py file,
</commit_message>
<xml_diff>
--- a/at.xlsx
+++ b/at.xlsx
@@ -17,10 +17,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <name val="新細明體"/>
       <charset val="136"/>
@@ -60,6 +62,16 @@
       <sz val="16"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="新細明體"/>
+      <charset val="136"/>
+      <family val="1"/>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -81,7 +93,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -89,23 +101,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -121,11 +148,29 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,514 +549,1574 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col width="7.33203125" customWidth="1" style="8" min="1" max="1"/>
-    <col width="14.33203125" customWidth="1" style="8" min="2" max="2"/>
-    <col width="14.1640625" customWidth="1" style="8" min="3" max="3"/>
-    <col width="10.6640625" customWidth="1" style="8" min="5" max="5"/>
-    <col width="7.6640625" customWidth="1" style="8" min="6" max="6"/>
-    <col width="15" customWidth="1" style="8" min="7" max="7"/>
-    <col width="11.5" customWidth="1" style="8" min="8" max="8"/>
-    <col width="39.83203125" customWidth="1" style="8" min="9" max="9"/>
-    <col width="15.5" customWidth="1" style="8" min="10" max="10"/>
-    <col width="16" customWidth="1" style="8" min="11" max="11"/>
-    <col width="62.5" customWidth="1" style="8" min="12" max="12"/>
-    <col width="27.83203125" customWidth="1" style="8" min="13" max="13"/>
-    <col width="30.33203125" customWidth="1" style="8" min="14" max="14"/>
+    <col width="7.33203125" customWidth="1" style="6" min="1" max="1"/>
+    <col width="14.33203125" customWidth="1" style="6" min="2" max="2"/>
+    <col width="14.1640625" customWidth="1" style="6" min="3" max="3"/>
+    <col width="10.6640625" customWidth="1" style="6" min="5" max="5"/>
+    <col width="7.6640625" customWidth="1" style="6" min="6" max="6"/>
+    <col width="15" customWidth="1" style="6" min="7" max="7"/>
+    <col width="11.5" customWidth="1" style="6" min="8" max="8"/>
+    <col width="39.83203125" customWidth="1" style="6" min="9" max="9"/>
+    <col width="15.5" customWidth="1" style="6" min="10" max="10"/>
+    <col width="16" customWidth="1" style="6" min="11" max="11"/>
+    <col width="62.5" customWidth="1" style="6" min="12" max="12"/>
+    <col width="27.83203125" customWidth="1" style="6" min="13" max="13"/>
+    <col width="30.33203125" customWidth="1" style="6" min="14" max="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1" s="8">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="32" customHeight="1" s="6">
+      <c r="A1" s="10" t="inlineStr">
         <is>
           <t>#</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>seller</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>buyer</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>date</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t>quantity</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="10" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="10" t="inlineStr">
         <is>
           <t>unit-price</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="10" t="inlineStr">
         <is>
           <t>amount</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="10" t="inlineStr">
         <is>
           <t>item-description</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="10" t="inlineStr">
         <is>
           <t>pk_sender</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="10" t="inlineStr">
         <is>
           <t>pk_recipient</t>
         </is>
       </c>
-      <c r="L1" s="5" t="inlineStr">
+      <c r="L1" s="11" t="inlineStr">
         <is>
           <t>hashed-AT-info</t>
         </is>
       </c>
-      <c r="M1" s="5" t="inlineStr">
+      <c r="M1" s="11" t="inlineStr">
         <is>
           <t>HE_pk_sender(amount)</t>
         </is>
       </c>
-      <c r="N1" s="5" t="inlineStr">
+      <c r="N1" s="11" t="inlineStr">
         <is>
           <t>HE_pk_recipient(amount)</t>
         </is>
       </c>
-    </row>
-    <row r="2" ht="22" customHeight="1" s="8">
-      <c r="A2" s="2" t="n">
+      <c r="O1" s="11" t="inlineStr">
+        <is>
+          <t>sum-of-HE</t>
+        </is>
+      </c>
+      <c r="P1" s="14" t="inlineStr">
+        <is>
+          <t>homomorphic_original_sum</t>
+        </is>
+      </c>
+      <c r="Q1" s="14" t="inlineStr">
+        <is>
+          <t>homomorphic_total_sum</t>
+        </is>
+      </c>
+      <c r="R1" s="14" t="inlineStr">
+        <is>
+          <t>decrypted_original_sum_hash</t>
+        </is>
+      </c>
+      <c r="S1" s="14" t="inlineStr">
+        <is>
+          <t>decrypted_total_sum_hash</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="22" customHeight="1" s="6">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>companyA</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>companyB</t>
         </is>
       </c>
-      <c r="D2" s="3" t="n">
+      <c r="D2" s="12" t="n">
         <v>45543</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F2" s="1" t="inlineStr">
         <is>
           <t>USD</t>
         </is>
       </c>
-      <c r="G2" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="H2" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="G2" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="H2" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
         <is>
           <t>Computer package w/ cash payment</t>
         </is>
       </c>
-      <c r="J2" s="9" t="inlineStr">
+      <c r="J2" s="0" t="inlineStr">
         <is>
           <t>4454349186393139520546745636716177895575862991839022462300052187807263520181547644630694076804606406910490795374102098658221664891588883149822925535400041697375213676801730870063049479459092515273563345378258491364916424402006466229547099317274246326974466787922807316790295956678153458356634939317768545331127736942901083131883545189878280282007088760492082008806289101712183594834545597988497584538885987627720754062259194952511413952470325660737731902664590002857958469071066473709492806549916843742336795698906504029223890614007995993674947963627795229617167450353926104730454954925846993580096257279400435825164039043261637781837789238216391041938260148790642612524238624190592440080208421794562572785838145213930456088474660266171511884890015814346374815942477675151654180143227162361778651581636015930775299842751123891156693697188045480487837548572591461509149828942074146910748003616372391398698214850872243962229069</t>
         </is>
       </c>
-      <c r="K2" s="9" t="inlineStr">
+      <c r="K2" s="0" t="inlineStr">
         <is>
           <t>3162244168983506277775705887871528840810894767853449323594321530387186331729308073920038371402879331340133252438033498394199532642125184006644737058644984051971655294222581652907912945387605440356321141061037936870539002045744972609745200108562518791455119291603594211201618270789100641722463506068463583532866970076154660576384530497507776308862976979526871819895210191532758498999320117714724267167067676096815491003323394272165440789934015937644405081833841293769563446407451824011147839899743548740214819999839843622549400649997303767295464933993226156812514503431628772460784688741657514892607251282172743902815752869990888138377651679787340515740742782787771588566363149530458459684146834165809909969433282927491954222195363347522589292747263860601616011096095062437294560199169739343849182683732945381000454339714649186830169094613153321907454776978064150105601009111785729356443838576978399465495221918248362753534699</t>
         </is>
       </c>
-      <c r="L2" s="9" t="inlineStr">
+      <c r="L2" s="0" t="inlineStr">
         <is>
           <t>79072ee229f9ecdfd4e02fdb1107f5274804ed7ba082b5635cfdd0ccaf5e721e</t>
         </is>
       </c>
-    </row>
-    <row r="3" ht="22" customHeight="1" s="8">
-      <c r="A3" s="2" t="n">
+      <c r="M2" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 9967596259580906362018197599029464488168344016863968492527884101496549090117458768737188335261371733795858162617830283708723931118175794745245464344615342017246669609287618226278613322737591037592818582460965977992503030446980162131581345669191950835624435474697898351692657377091533040780991684163226119780413737458665192369253948859872732757932422322676052490609919767471654656024250967937995341706697868218558964805527533050317380893068079708989641585696174353550834090800124275908598367080551529210074921907744863592529845890796941301542499967535357270862362267203972751083301269674318773148239506261284560059221224286220820358433491324979011252354825543237694114748730617469525177537645410733479140725675474112275705258943227346544531938680170503088185797695824273005255143402451380943790887375679842574121165368338076893992397312069341716368980618612100752069971689045016941812622759697313265396643176410198460709757987900869907264445621991803232361438698609479541848067146299840589936706592225836156211746834016811238069854008268799619751532394620294216191273470809952475132813439180464700664559559472489357829681276826659934901910550280516664626382488188203567494464239058897446693483607891818079188268789700022481151640387809176712029330571598856221545831871573708189889186086361762559947779175406589458271292018863320542242949096200398559247976502148035886405682514221981053351918236392418955275033088878538332642492593928903642610555915452590677161514801912471657266252330437729126553145925855926615685692777420278930818604347262650617018075381952105771524239660068432326095205506025019807444454105131242551789008338763222068962370874939222072706581112780915840228547277317850540822846734545381169305175208665651258650068799354010581264890340768837418872598862623677876421478930906455511295083885124479718034359062048385289891817775370135, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N2" s="0" t="inlineStr"/>
+      <c r="O2" s="0" t="inlineStr"/>
+      <c r="P2" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q2" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R2" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S2" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="22" customHeight="1" s="6">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="H3" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L3" s="9" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr"/>
+      <c r="C3" s="0" t="inlineStr"/>
+      <c r="D3" s="0" t="inlineStr"/>
+      <c r="E3" s="0" t="inlineStr"/>
+      <c r="F3" s="0" t="inlineStr"/>
+      <c r="G3" s="0" t="inlineStr"/>
+      <c r="H3" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I3" s="0" t="inlineStr"/>
+      <c r="J3" s="0" t="inlineStr"/>
+      <c r="K3" s="0" t="inlineStr"/>
+      <c r="L3" s="0" t="inlineStr">
         <is>
           <t>c7594c4277d03d892100c1aee221ea56d4a6e3630e1a692aa493b29c5735f8dd</t>
         </is>
       </c>
-    </row>
-    <row r="4" ht="22" customHeight="1" s="8">
-      <c r="A4" s="2" t="n">
+      <c r="M3" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 12480165976769163183856768494501321876975969755764187156507584403100436210124238997828128084302543186904360764706825000428836749238242104799018716693189055232867906970238730646911309206027398218198717657176097702580271637313757008021426641799874276281005002168062995110488773729144697213733182401519431321859591721107599552501930868271180043845150338969004030029233077386908506909390544954831916251527872325303147589349407853781295538805579044259261001029950604373883803185320320090537963242168413724825197384100981663541923582938821759215461333318335396729835693012045898140826191674047570706473547610257650553277572387057635324483165201484207872691867658531326333061161577824260526574603153989375744880017850971600299646397994215850190346771793488530741679660639826795572603486079441101200911714676421108078243295513398521965496433684197642124449557377875733879270620502629426818405942777372117518899630906259581442135606641132514989592101501102838242512896929888884497997171032465089542013694161609270114351603394531655965277070521347711015506308618718812274492969347870384617386454890093421002819241351108097129156415216339991135226325261745874054036950167625268246049346305669580215281047241483817093960692926188937437105515907689923900197110244349293814975179710674257657354906536759353692195296236520955526105151283061707847388243234538662716049389558375666385858542295119115944758338136675731429532477279624371429225465497893191200617623830067363956198944830808685897728623122134975659665666368704259697514005304444677693403884992672067523839340476543453253667927832818230554198962964704906855304263338687614194724753056807868866747031348572167778566258958015564525022858673838905530116266559978459275446888548487601904285005055607714631663390663705841607352735101930072590790508964696351445744481319973855526420324472563003266086753609304117, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N3" s="0" t="inlineStr"/>
+      <c r="O3" s="0" t="inlineStr"/>
+      <c r="P3" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q3" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R3" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S3" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="22" customHeight="1" s="6">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H4" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L4" s="9" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr"/>
+      <c r="C4" s="0" t="inlineStr"/>
+      <c r="D4" s="0" t="inlineStr"/>
+      <c r="E4" s="0" t="inlineStr"/>
+      <c r="F4" s="0" t="inlineStr"/>
+      <c r="G4" s="0" t="inlineStr"/>
+      <c r="H4" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I4" s="0" t="inlineStr"/>
+      <c r="J4" s="0" t="inlineStr"/>
+      <c r="K4" s="0" t="inlineStr"/>
+      <c r="L4" s="0" t="inlineStr">
         <is>
           <t>a7762c02c58121dc861341b0dca1c33e5c2406f81cf32822d2848e4729817f03</t>
         </is>
       </c>
-    </row>
-    <row r="5" ht="22" customHeight="1" s="8">
-      <c r="A5" s="2" t="n">
+      <c r="M4" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 19236069317314118285224092452384611712727240199118016628768499916353899663722311167221055993638560609072395006611567644897295875166216904922420727173969978284694018737609411745616918768868699253548222109995355700436862369873777761038254719581711075378333910013948465587315541215004755956127088168627461947121353433213915749740945293804727479930984827688226102548819769123725157408101240949858942568934954074688521897181278519746407660409947379848384838345983710549130901115413767463694798671579418168999868025560202878921890233055750096046982450334493154857503495669610802648621782660944273336126400748641972452068962789204764205264471631817492843310950437990315991209814787753370870548828791560279673774267024413718619434372698851135586932460926239575881152408373009691786888164577906100375695318340126736902680705014910020159432424730295387825105328990753301644374982816508241646248787476056825966120008190348385363915399121639890458227916705341323943568680343382909878576817383517727826082553037957794811957993893374532793215752239509409682126237129796966215070740796261759131534247097418094097984066113607454221205580737765790606665503278960315792565809196835269937199480562398697992122487511325190748382096345920115335905082224252278752535123519643823841353109090628901424646575175756167161555875303019024333256853685666589910517965849595627080417029454189866051971925291175823152415201519376449591634949671363570689588889027638753255984075531974910422351956041934888074608682672296802423714843540089770752707438224347609462984645000147414192030020098814888292502083243085452794030528886847090981506835065452543508532826273792028424588650822202135276651616942872051727760162568138393525935214132799440536024299328593659214880306313117695398428637094424919481105402280047080472913849166781542716960074133459975370174903904196724273963343416971521, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N4" s="0" t="inlineStr"/>
+      <c r="O4" s="0" t="inlineStr"/>
+      <c r="P4" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q4" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R4" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S4" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="22" customHeight="1" s="6">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="H5" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L5" s="9" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr"/>
+      <c r="C5" s="0" t="inlineStr"/>
+      <c r="D5" s="0" t="inlineStr"/>
+      <c r="E5" s="0" t="inlineStr"/>
+      <c r="F5" s="0" t="inlineStr"/>
+      <c r="G5" s="0" t="inlineStr"/>
+      <c r="H5" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I5" s="0" t="inlineStr"/>
+      <c r="J5" s="0" t="inlineStr"/>
+      <c r="K5" s="0" t="inlineStr"/>
+      <c r="L5" s="0" t="inlineStr">
         <is>
           <t>e7eabba8986168410de4e6921474b12859cfb2110b7f202b3d11b5f0f21560be</t>
         </is>
       </c>
-    </row>
-    <row r="6" ht="22" customHeight="1" s="8">
-      <c r="A6" s="2" t="n">
+      <c r="M5" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 9508019881338126896087355645973153309354333066492518400908485203884739853333664653675477744357784004863850933694933528100315662059476166089396476297372695771795436252166816887326072186984656764269261650237896403491549050929441692336615143341383097362574935277171287775575295437791258872168198819443847843147955940511512544288880073479477668396346749316905188102374744756901232882443582580941763560548335567575761605148253552826869676948330223956514548361427715846280879589601509459699291946740751592988948778335006645863019633265620663133546974169433908426921011035422362978093599201004508101696346722248562854494189869920078121658087432583871429703770391154694189682228292500408034333295153356819733310810390154976910424872800141064476904794260310369922082541193489914591749473072036965022051154993045932012595974361836341704477255355155831387785740755554150592361839965453020081628991060812285327454343498571034380316903331029334116114908625300642608258719025169440114635034475273432347320459179203222096987644937502006083311101436006580630402641829195600625295152755778213480537116077255989033873936870114242884968629293329375640454946113005110310835549309285939703769287559467017262577320212845705435462123245478102166844532772168069189495224073858057304070749348755579462401952565646661495477391838847889124506987828587112500715493966717576079067028609963823961855457191502185445729201858816808529940272655594979154669399907878478145258702397351323090459546112654923849236016714178832432386035424848752776572452471634269631533853802901796694088964523290285867272254622673471630752264119949789506222465416495694566150005943719457100725285701323062396067860636142008085628762975505928090045704004932710429482111896007999860456612569706856312218736945472333475717710534903939232667811480700814338328154073136739680782544137954867222294040284890285, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N5" s="0" t="inlineStr"/>
+      <c r="O5" s="0" t="inlineStr"/>
+      <c r="P5" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q5" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R5" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S5" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="22" customHeight="1" s="6">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="H6" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L6" s="9" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr"/>
+      <c r="C6" s="0" t="inlineStr"/>
+      <c r="D6" s="0" t="inlineStr"/>
+      <c r="E6" s="0" t="inlineStr"/>
+      <c r="F6" s="0" t="inlineStr"/>
+      <c r="G6" s="0" t="inlineStr"/>
+      <c r="H6" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I6" s="0" t="inlineStr"/>
+      <c r="J6" s="0" t="inlineStr"/>
+      <c r="K6" s="0" t="inlineStr"/>
+      <c r="L6" s="0" t="inlineStr">
         <is>
           <t>ef6430200577912dc09ea0557c1f214976a0f1b5341253318c3b1d4547808bcd</t>
         </is>
       </c>
-    </row>
-    <row r="7" ht="22" customHeight="1" s="8">
-      <c r="A7" s="2" t="n">
+      <c r="M6" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 10811793938928041535218643967180738408418264841080906674155715930266522657762229932274873370485604348326909926288701782970423248404128555822883535678338886989917469115139767587358363296415017374920407930808489646320714828660841212294654184725984787466254013122474969514355112553253386771484804323935845967818123878900059282700311848625546860518840108636347860731892908871648933847153496084596445147060080850654376762005174994077317291321311926663116546387539185005364920444746432767300409480468771088274876871992113446185938619951883135785744670214221447716891618492410189007146796284892488851183217645899437419730082914527070146871750771167357467386844042528679507157437454718167907214791302870272779934357678162867978819805795597511321252363337146792734395181383391463147409759923411935977359930640726255660287968221856598159014039705534355827254589834990233061068625645582765447775193542860781411036379653607099238690551934915619167056715082976533813928987467402278551598959228849777688300646918133286341157695653286417456107834898937778778037037215129011463228367320468827403812260629563285438925885348357752874080463516509250821046875999298954735929711064615111107487232500498235512191318342740018038078358398817374728506576831772760228323550457167206115483866089783113169302597063737311583985158163726954228181969375539947926052906943463992784529996705793526839271619509466463370761870375778731579339476905975678879526214816613706190769257231738348049203067753946864757939099433550593864189626419609652767670112394561687835156375493340892335493134927364428155777418628067163024374184949048990195272206815317134111795253076740319840986068431002811188379154584869972482735318375517451376449440156375506434341118877556267166069174557482607910908238970417505914202255467597147422339050392583241400014615070178375340247701295277165711432241822341047, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N6" s="0" t="inlineStr"/>
+      <c r="O6" s="0" t="inlineStr"/>
+      <c r="P6" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q6" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R6" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S6" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="22" customHeight="1" s="6">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="H7" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L7" s="9" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr"/>
+      <c r="C7" s="0" t="inlineStr"/>
+      <c r="D7" s="0" t="inlineStr"/>
+      <c r="E7" s="0" t="inlineStr"/>
+      <c r="F7" s="0" t="inlineStr"/>
+      <c r="G7" s="0" t="inlineStr"/>
+      <c r="H7" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I7" s="0" t="inlineStr"/>
+      <c r="J7" s="0" t="inlineStr"/>
+      <c r="K7" s="0" t="inlineStr"/>
+      <c r="L7" s="0" t="inlineStr">
         <is>
           <t>931f3e22d809dd7fec065d067bf316757f3af2a094eeea5ddaf425a9f2454d35</t>
         </is>
       </c>
-    </row>
-    <row r="8" ht="22" customHeight="1" s="8">
-      <c r="A8" s="2" t="n">
+      <c r="M7" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 4796017654851543903706611329352507843333304803134872418645189946846970801062425921168388507295333681051252214611529697500184044267274660894258158249784216412661703335601606754176271311905966402683816360551689817675653103480592954176555125123158586150163388205961386504299772201863398021640024179806987065868413792381732984304139713933523463740685636008888214810867207365277043432840435899725401785142013264726247725520604702996041323435059840264475942323231173341411015703355865916783174519769401136095445843892770336924670968067141607004296760096973438242793423734901075638694458027841185374416730967746778607998122146473513745211153971768523174064966088612442169776495704934849287648086229499584537259626335997339253755755601343100704593759987717967655384158058268557290820684249168489931678353170179441391068664725491437368175090527224969865370096994894364347743370779456741560583013557557838178921419920138051886523734655651334677266225186076496383249744303872767781418286065124512705108347870394463955821118476094504190402289009492551001230539617561531098761577422850704284041222650547686378642520971514465992435257933929992077204654690181414730289373584900145389112934740111130583160009527308137122385944688209819447892464827678414203542100910978485242023639840681992376621499513673254686036684579734252527988269634594150930558023529531881272250469604597263438108866010389706210088999632828317124839080017443413615983637384163283234129834976173946508713469290630478382941704746371997654062928972425352844213719140964839542732174007824137055945574184370239330862231169839397943890582025119367491537809904641268052932568937880773477566711535599663333704590968863675355965536175033979698718534622255149889419352667773011588526810408903292581991764404429280230232137065874836976482396585598308579363587515327879206652052976182831692859369073177393, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N7" s="0" t="inlineStr"/>
+      <c r="O7" s="0" t="inlineStr"/>
+      <c r="P7" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q7" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R7" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S7" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="22" customHeight="1" s="6">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="H8" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L8" s="9" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr"/>
+      <c r="C8" s="0" t="inlineStr"/>
+      <c r="D8" s="0" t="inlineStr"/>
+      <c r="E8" s="0" t="inlineStr"/>
+      <c r="F8" s="0" t="inlineStr"/>
+      <c r="G8" s="0" t="inlineStr"/>
+      <c r="H8" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I8" s="0" t="inlineStr"/>
+      <c r="J8" s="0" t="inlineStr"/>
+      <c r="K8" s="0" t="inlineStr"/>
+      <c r="L8" s="0" t="inlineStr">
         <is>
           <t>1940888865c7b8b797fa45fa89a0c0b7206ab8c4aa8333a30e4e6106b79f4f70</t>
         </is>
       </c>
-    </row>
-    <row r="9" ht="22" customHeight="1" s="8">
-      <c r="A9" s="2" t="n">
+      <c r="M8" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 10188526448065483228673535475473364911884406321983785760970510331648324647609499094709609690526596083647548645191376294488691190576838767337312088943532323394474860505309560701296109652080663441144740359856611015711204021842431567680274192081298964850866019619878798649179286850729937146234572191829212915569092275722439939516237072180432719219221417958316360654968800762710918224304202200900510114692859279775517093124405946640234697524221463276188932368429998783543470271019326248170534555959974376264708859606393669238733577625333859890662635501400992598069574337088349940822086530884237413775003298981081427775687805673016404131709822570836125760850848852101354679735269336175264697328131423311041563449461946138006241575605860338438490351795635158506605677252877395621868439348971874562558504939510489597449713691560396330909479324713834954165907572973617211492777412385002549063416761356040978786907038083488609598594527705832702936459613114872256547031621080172410778430202995536154496737799694762819301071462904285146052580953317481277449852217978720730414672108336984674596788787128318672969208368618940046825765632505292063761396561231164159817207199744668544128072539913169195563749967734293263875939550620767970780196118541649256526079691274695702229217831923497970416337313908780546340963825542983799966120053493893003287726492541404152482833284122327615877188203428083377783169563343093970881029198027589326879198516488852728352336185740403516994808585971060680850134488643640055127974172998481086374975960194246092345581715605127173560447704267297298318329560196152486858158840050514742213152959176115404563784513296812364745558360026667289194818698530684091168277664575975000975746416307755905223946064849750690559977242443010811726266950654082960888533825706568508042730875230900593514509410507327419370877726537301538506355259855551, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N8" s="0" t="inlineStr"/>
+      <c r="O8" s="0" t="inlineStr"/>
+      <c r="P8" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q8" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R8" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S8" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="22" customHeight="1" s="6">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="H9" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L9" s="9" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr"/>
+      <c r="C9" s="0" t="inlineStr"/>
+      <c r="D9" s="0" t="inlineStr"/>
+      <c r="E9" s="0" t="inlineStr"/>
+      <c r="F9" s="0" t="inlineStr"/>
+      <c r="G9" s="0" t="inlineStr"/>
+      <c r="H9" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I9" s="0" t="inlineStr"/>
+      <c r="J9" s="0" t="inlineStr"/>
+      <c r="K9" s="0" t="inlineStr"/>
+      <c r="L9" s="0" t="inlineStr">
         <is>
           <t>564db8d17bf2f8f73755b75510ea86d70967737425e6a1d8e3aa8c26da009183</t>
         </is>
       </c>
-    </row>
-    <row r="10" ht="22" customHeight="1" s="8">
-      <c r="A10" s="2" t="n">
+      <c r="M9" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 1140156654146213752729927661356455077768313012193232169934680120550914480065196757102019669486821552386488816395583909244675184215573613893227922093697037814662667901229489398758127861913126856339567556921554312559628713570646752014350941299718694613271493893092745688555636898556215331301086475911494424698121192819643316129961050835161018885122792802092920429449046842430181001634264130578608047570810978759842467921171790260787484451882927184857747049646395358292033036977144315524932663289828705679459845122201552170414479825889970806584166739184215224323188214335384352375475998577800442244821928356070607142211494657291173986121187357609816151089305212630324155653592257736622832609293502767724369978421844944221126406082047812568934011938474523905452141160927911326774122054911572518024770641411403735477999203852524660827225767926721032388250408788113209074615598130669394906307355662239775235253153806346121092893035090167427676199867377899949934518379686841253108837553858916050457744772452046904956536446128471260977843880451502906279901229840195227691780313029340865388693579292328116092562259446263850958465709549212036890187780187722741111759932022330669353753416995203336731935115449576439526148394683831943537982674533912638740279162521845210258030920256529169446233233827547395261303620102226442540402843889719221640488838743759903148666680731573255012736379071199418295045584637209584711677219089614366886499618706716632451913003890062671568077546253796847771099973727660994938524906307179811333323739811425626632002685175331419048235198190122739837302746089721613612125289134499747735861002905195728925863492002904802579937983101688992904159720323688335102497295114831008299493086595434626892479477553956418505546968959533838047978314384510926194118848789586835419734182988612915924416487431649885497121212843237911685617932785144, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N9" s="0" t="inlineStr"/>
+      <c r="O9" s="0" t="inlineStr"/>
+      <c r="P9" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q9" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R9" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S9" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="22" customHeight="1" s="6">
+      <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="H10" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L10" s="9" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr"/>
+      <c r="C10" s="0" t="inlineStr"/>
+      <c r="D10" s="0" t="inlineStr"/>
+      <c r="E10" s="0" t="inlineStr"/>
+      <c r="F10" s="0" t="inlineStr"/>
+      <c r="G10" s="0" t="inlineStr"/>
+      <c r="H10" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I10" s="0" t="inlineStr"/>
+      <c r="J10" s="0" t="inlineStr"/>
+      <c r="K10" s="0" t="inlineStr"/>
+      <c r="L10" s="0" t="inlineStr">
         <is>
           <t>fd7d780ad09d606416d5c9756b9946e1221d86fef262cd2ddd93af1ba21306fa</t>
         </is>
       </c>
-    </row>
-    <row r="11" ht="22" customHeight="1" s="8">
-      <c r="A11" s="2" t="n">
+      <c r="M10" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 13572624628710793738768882887713339208195620145487264455250446445695794826659300028613699353042051652789636920284881453583237357407406713735833140356749337460147093893582926864668807732515728549043716334940285122610978343501145475701249179747164965383172160044883140886238765972341645290463762835172431531234879276029191724160612968589001507908353751493191607453258408323200110612838309994989210703363222207398518644892593417379371858647401530849111094685742595732149342831640283823675681926329749266321446345723793895922275701560622034499877978122808976949984996698654716046123194721359913723566690688408610484392724578733620730546539618324678264023059108262718885341025327825792542788529473855964530307976371219125689023918156350508583470801541606223253757763501603081686983631281335214883130566467183463215656848498035532423801582230367887915043431495624346026744074809370865087035485369359532580343925338936570220811670571850462065119099394079518644034063855309687139087516567722860129910525288260212106050181056177096289205790468435882929397413966142519791438984325327330304301700422082390882406706948119237967627315670349786924259467797057658107678957886857303309252804790166647873624299705427584148802987547096899428759458702551027280677389696008493867751518425421657575798645793887345107629309787569285101093629863770141927902512781952740500588850026823516191211326341936332287319561496999966170045075893872896140650958379825468619604878770631988937878646286544359458870517864058090418401258452778681862347273340159085890561598359701716553748933465303389872103786946884521533207281635562953746918526524617757278871611461541075467249037986778998804209724897687704242594881442435831335809085000561696902948488417759912034426108840051382625857378990989943800304796296667303049758385725367720263541901660194718302320716010289387542888719656652058, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N10" s="0" t="inlineStr"/>
+      <c r="O10" s="0" t="inlineStr"/>
+      <c r="P10" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q10" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R10" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S10" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="22" customHeight="1" s="6">
+      <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="H11" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L11" s="9" t="inlineStr">
+      <c r="B11" s="0" t="inlineStr"/>
+      <c r="C11" s="0" t="inlineStr"/>
+      <c r="D11" s="0" t="inlineStr"/>
+      <c r="E11" s="0" t="inlineStr"/>
+      <c r="F11" s="0" t="inlineStr"/>
+      <c r="G11" s="0" t="inlineStr"/>
+      <c r="H11" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I11" s="0" t="inlineStr"/>
+      <c r="J11" s="0" t="inlineStr"/>
+      <c r="K11" s="0" t="inlineStr"/>
+      <c r="L11" s="0" t="inlineStr">
         <is>
           <t>77011919603df6e6e1ff670c4951bc53ac5ca79912e44bb0d466ad59538b1427</t>
         </is>
       </c>
-    </row>
-    <row r="12" ht="22" customHeight="1" s="8">
-      <c r="A12" s="2" t="n">
+      <c r="M11" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 102156740720167039686845840366030794934596545428079519182721683880726141866938628668319986861732301903474682811586881404895806562712864083596516602317206377719825644012985460912392135374931445793252246460486848754434864918522859540960082777840931297451569335671172547279838502817965197384377167230468369485769907353518927041633365739508052250798810838338975723738229577112222144860608129053819477222757061833619764990302609978140438520621281201181919414801486149807391298539427044111701791254866646445781005944020784217055633810111792939857380953729438451777036392141008154844424156167648726765077632311084233333390041114054132301620709505966748142450836204506008315028062262293456597388205347108610465597251008244830814596711593147814420790040714870991934647412116929975919284259044126655457492318409613939493248311643535631960325124335223247967817833555126097578232357212835346456919143847273824284187957157631430741244388917836625534301426800408210849969922869911427015473881674586032732824185009399233100085402487895142378668596593351357306299450238836447147857520539986417975019112727149719172063140314226757526522403253113679833858659475839570172391775641495528008633081152901753688379998611372550386668301076690772926672814983910114233352624604013144295099578894676744597051392318049094748505631835728701100137876730469572643401419864320130251175505637400440486254754917298902718048876971786085847668995147342247708148756971702371126673868087113466911194061070229673259868056406055954156252362271360402908220670166991409157320426369733039195909545649048095760586236127665833286429181691956551766949908288516316992426195650465445906988941577331161739469038985041003714543487158437683874366181394729447263003172854736545046078316484821404743416236882088454947794334631886772104916899615682748283539565016020206765270169334950420961373989683345, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N11" s="0" t="inlineStr"/>
+      <c r="O11" s="0" t="inlineStr"/>
+      <c r="P11" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q11" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R11" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S11" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="22" customHeight="1" s="6">
+      <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="H12" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L12" s="9" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr"/>
+      <c r="C12" s="0" t="inlineStr"/>
+      <c r="D12" s="0" t="inlineStr"/>
+      <c r="E12" s="0" t="inlineStr"/>
+      <c r="F12" s="0" t="inlineStr"/>
+      <c r="G12" s="0" t="inlineStr"/>
+      <c r="H12" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I12" s="0" t="inlineStr"/>
+      <c r="J12" s="0" t="inlineStr"/>
+      <c r="K12" s="0" t="inlineStr"/>
+      <c r="L12" s="0" t="inlineStr">
         <is>
           <t>ea1a209d740d7d30a6ec7f1e2408b4353776f78b7f150501510da10ca38e7960</t>
         </is>
       </c>
-    </row>
-    <row r="13" ht="22" customHeight="1" s="8">
-      <c r="A13" s="2" t="n">
+      <c r="M12" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 12010311695308902196447965315043911475165731999106586312090067397021728657630486182126835094454036166085335759292544633569076163408232426632187905426930813163307200639811333101904448381873224311846731791291157355025361425654306767149486537228935698675978787022518141783962016439968108519072119273006190312494717395669129469444208234848827698592216483487421441207237332410042883172690129134688362589087826311063136238430973482251691888459441706061341338798784773178254460086659964008750409434991518029113448223864271916386244675365546480844366552852808841082222955795180155665753557240565028810111765870780530223842095468249360504743928667188775607805312837852035038896646295926896096527194313720728247051108136186464432028105579866245617960805084391582166257488411473624052071614132441917217148404096553425605840091473859233839982421586008337989215890269193139361768713589532004494036166052989011910060385826681274316493810024374907188310658410715301982756799795488818266280631782551353754743668964655374853363529517508540279767975320808235107482599646110587778961861411955129463578844532634523953905553395373341941194421320709302464752302856096157500526335430780530891201880064211418049369399834057375990134869683403513743443684687546388348809391990091217309964642242709820090659070780792781185103469558927374757715891876676553279317114288925219583278614073363496640136974231641659289124901281781375510115969765464997234056868106156111654942127968833014454726015046255789535275244497468618003328763474654583604971037982661894130716451918715757064528639210165783835002705410582340220263774927953797581935758228653028291554183013766935123928658661565744120284325952013424662678845075655836024878331472305539369083858019870306497196409624387547325828009038722548836236950291634412267175739595364118543650247063505306211690846606084828500742693088614648, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N12" s="0" t="inlineStr"/>
+      <c r="O12" s="0" t="inlineStr"/>
+      <c r="P12" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q12" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R12" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S12" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="22" customHeight="1" s="6">
+      <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="H13" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L13" s="9" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr"/>
+      <c r="C13" s="0" t="inlineStr"/>
+      <c r="D13" s="0" t="inlineStr"/>
+      <c r="E13" s="0" t="inlineStr"/>
+      <c r="F13" s="0" t="inlineStr"/>
+      <c r="G13" s="0" t="inlineStr"/>
+      <c r="H13" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I13" s="0" t="inlineStr"/>
+      <c r="J13" s="0" t="inlineStr"/>
+      <c r="K13" s="0" t="inlineStr"/>
+      <c r="L13" s="0" t="inlineStr">
         <is>
           <t>68ffec0273d5a07a3675e34a079d7cf208474dea9e1233dda461f157635d496b</t>
         </is>
       </c>
-    </row>
-    <row r="14" ht="22" customHeight="1" s="8">
-      <c r="A14" s="2" t="n">
+      <c r="M13" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 15406241686599372575237279049868930775824680934950882405834359991527320792658192400226367484397269828397655013509449396796651881033659452743117387675799085397884886696119969249044736793247206534493474528471480811501278798399318160220750318841286641186469222156539773356643199185793336771621508266037756628210029170998075984583910411453568104997737552258010580019371805623278337391761520077120921209321941100073669873384638322605433290966541740108467968753657995119917107871782195580002364497142245858970733559736210528494530910067313936703387743887789511303463177833550331419952694400748045798319452596516949977542840926630459984623745222106188062554246754184025450417314109254188282278595043172305029446626309013976050197590832633144623113103733674979780658578021086754223389128046904141441160764900802057834874950769410238391821433532075859628148658135758635541565270151315175953909220080425613939009416966823635103621893119039480888137408151573921371669330302447702532093585310490901003905255336259783385421878241292755634020712567106899004605579126377549582722072143048886714887482410405651415503121236792094569736277263115966717826895101039095891549572264928518760435344620594993330505951618034436010244009089231715016791564721042852445808744190201328073765621749369584706842515064822163940491883660154414603950787670010184645387522010623172854643682074808721774971284974988804288850419246509556678662388287822991796208016148440679401412157070178113463798065058237095572142526633924852316407772184884385023063556513758360111933276990146341472234444263491610824613698918998963055349929980193876985936656786252377438590395396425849507038660353383217457774915310300356268348590443194484536260169414482154628723627471750970867831213487947724829455989193085181706444970931900690852503895808196168423600369612928326386284682101399581879171352924634814, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N13" s="0" t="inlineStr"/>
+      <c r="O13" s="0" t="inlineStr"/>
+      <c r="P13" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q13" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R13" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S13" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="22" customHeight="1" s="6">
+      <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="H14" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L14" s="9" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr"/>
+      <c r="C14" s="0" t="inlineStr"/>
+      <c r="D14" s="0" t="inlineStr"/>
+      <c r="E14" s="0" t="inlineStr"/>
+      <c r="F14" s="0" t="inlineStr"/>
+      <c r="G14" s="0" t="inlineStr"/>
+      <c r="H14" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I14" s="0" t="inlineStr"/>
+      <c r="J14" s="0" t="inlineStr"/>
+      <c r="K14" s="0" t="inlineStr"/>
+      <c r="L14" s="0" t="inlineStr">
         <is>
           <t>ebeb1a1ba33654ae0217085bc424d843059c0a4e88021ea00f49dd734bc634c8</t>
         </is>
       </c>
-    </row>
-    <row r="15" ht="22" customHeight="1" s="8">
-      <c r="A15" s="2" t="n">
+      <c r="M14" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 7805290938562741253820505627965605634022127562594489634786886686461800691316180018229650765189885749203569374324356764153144010626625332061067542714546829659331954170693413846188066316432870318936344484586621514715615511160393197262060933528061064462963733420980635943236304830391225252880302069228269343179107985414180780192216118924978244101607559203956016977879741820939447312287160166116070250993361776041087912939915825840187040979073857402450966497998492048069365049911935480402914027561232316232224585231354720533452366625860133094996070532701829386005291413864712081621656419525212572271214248261698148696310378770860624820263717802952618583742101071306370102330125367824572775183602296497278206772893270715201359556410441698475551215086500372187740713314881476561241145250724786266331135224245646379905455671513212034143084102917917908015662309235585314792850697615720098520712542311410068871611953309981494563085281993056054805896389656659917828094834844397072947428629414612754379050656065539360975262261306216976062922236491583308017330690880818581665738723042593687235161687030827671881433647925679428377317830038282128384208110116459210766202218484114413992240840213038609600103066757558912227246840721906940906800280994773724017819440256223247779147301884288958506437811836958704631820159693758022866213648094268403537933425576011896120539846362997068133859820586590023739260775109258155778224929024599247313859711836350505826045128939547474895205097727821034122051219744282467322647827848262565337887847129136107486098060129672514295106777173519994556440936569817978263164213053888415020536696824289654841606264647249013675889618753614425028547420643877999963867278893345048934162058265191400595449722486335412336397996555225899392498123314383823907263259893751802648821636312510597205130009827513479575904766087704227724732907150740, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N14" s="0" t="inlineStr"/>
+      <c r="O14" s="0" t="inlineStr"/>
+      <c r="P14" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q14" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R14" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S14" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="22" customHeight="1" s="6">
+      <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="H15" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L15" s="9" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr"/>
+      <c r="C15" s="0" t="inlineStr"/>
+      <c r="D15" s="0" t="inlineStr"/>
+      <c r="E15" s="0" t="inlineStr"/>
+      <c r="F15" s="0" t="inlineStr"/>
+      <c r="G15" s="0" t="inlineStr"/>
+      <c r="H15" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I15" s="0" t="inlineStr"/>
+      <c r="J15" s="0" t="inlineStr"/>
+      <c r="K15" s="0" t="inlineStr"/>
+      <c r="L15" s="0" t="inlineStr">
         <is>
           <t>4d5dc7097911807b3c1475af7d9b67d0987cd274e15de1e441d44efc0b6f5a04</t>
         </is>
       </c>
-    </row>
-    <row r="16" ht="22" customHeight="1" s="8">
-      <c r="A16" s="2" t="n">
+      <c r="M15" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 17566471392992160776674757347228484662664344845526272131747010514083151762216720771891612768701452763749877465131237348448057908828375851421023322831245661986748851233871636334133070809344803110210037405144013636803103053253194464432663889474201842155840261833976838222240360737303699664196019876010664392396798136722944250296037602853296578987707754537603692062689830290219568715532891070836336933743729232412378099028944197710730227135888459518791331483491053721033704514948820845446744103529285026864604735361113965740009913137651524606052909531244633453378903946537486871445037524898098786589292412679790347411163706525433226129202421955833408062812952193458645279770747211766466153938147566226085913934544642026202478394106217690945905818429275354091540129872351921978647027383787434000186962816871381175655251518389812662109552195095694441520223615820450218300317341158490348933084467442849307890965084577662428799586383682873219474914869986052384716622816495776251647998189106730008384718859975707940328098919981418134213716553641696582342575229739861907740078854591347822247341799479788651825047900597503107388981834014569534493463639012257736989837914596439164379113633718110440794433017253861192418402955498829951452596608798065489520671253928369207874002778262684580586160519799117975296313407357257434800932161265871624842777142980301666372848004093037434708257326475989643717072446336882413002548534664855773440706538669938176868817289764786316706155252885181712004649720617401871876169906664851422458243235884110619159788697446835280079222289604669480544829041038445043822562308541890544820385587000310536637194210180420188126873100435611723720836388246857273149039764094232379584505126438482217070605895970558435345788477671397931096526145758651117750393779724702339093623348606806048584132721699715865931208679886994782365517254697355, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N15" s="0" t="inlineStr"/>
+      <c r="O15" s="0" t="inlineStr"/>
+      <c r="P15" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q15" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R15" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S15" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="22" customHeight="1" s="6">
+      <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="H16" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L16" s="9" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr"/>
+      <c r="C16" s="0" t="inlineStr"/>
+      <c r="D16" s="0" t="inlineStr"/>
+      <c r="E16" s="0" t="inlineStr"/>
+      <c r="F16" s="0" t="inlineStr"/>
+      <c r="G16" s="0" t="inlineStr"/>
+      <c r="H16" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I16" s="0" t="inlineStr"/>
+      <c r="J16" s="0" t="inlineStr"/>
+      <c r="K16" s="0" t="inlineStr"/>
+      <c r="L16" s="0" t="inlineStr">
         <is>
           <t>0379a83785b1030135a797d73e11f763c6a977101d7fb514f2de4c9491dfc14c</t>
         </is>
       </c>
-    </row>
-    <row r="17" ht="22" customHeight="1" s="8">
-      <c r="A17" s="2" t="n">
+      <c r="M16" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 13787818838637803342985817917161462230174775267120614846401854301001318128224488278839478195853437074936334651253751500069877307505016948892099971464654080860075232182728133860398349114152763567306816891838149230463496438193235983722954704355419346041927043743586281554895819271198118692730800562225699515448029912344947192125667530242972147599169663646509552291498144470260485554311872049965802852776969771773891892828637320685772729017455452621592098437774610331071082309240767562447831417599538498377965304160297549770238477572204496978664885002862236584844820716437455288566204905277730171303585610657686669678753257515426985470256646147956831364273505490495117903406755971501667687537788438986501491937261955767946770180271523707052176345842401953243166194328909510820017829262142478488288613857667092601601968550953009609253060193806249016828072798253991403417803951959431731420762777424328878205064179112924010828708821294786042301053726323185354526692005443242616862632315441233057958993348988378141586911119450219191358922331838750803791248269241748960606426027536297430042241023297082640168926169628715998599453620681254783068745561138890625786547313592264169888172922943809514445322647599362648482056410119650686058172527356482338873005864013335082460314177275330937027750145491321608275771800584065738023641928126142770554029362523626265222089949419190157689878430166445952129073980157852313725272401795193327192896984555163451025490912239962138468622998781859541287793539667411124595256202396139993307295677151585173689213758746946052441862360347115337312297790451878396976307945149160817878707477431967447255135084882911054529608541235318005406504725442418271649971299841976958954178741296883183988347000815650667997822028131651102890928081172561779520326253149108320426566132810337869990550542892118004448155393966811318470790094586156, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N16" s="0" t="inlineStr"/>
+      <c r="O16" s="0" t="inlineStr"/>
+      <c r="P16" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q16" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R16" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S16" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="22" customHeight="1" s="6">
+      <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="H17" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L17" s="9" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr"/>
+      <c r="C17" s="0" t="inlineStr"/>
+      <c r="D17" s="0" t="inlineStr"/>
+      <c r="E17" s="0" t="inlineStr"/>
+      <c r="F17" s="0" t="inlineStr"/>
+      <c r="G17" s="0" t="inlineStr"/>
+      <c r="H17" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I17" s="0" t="inlineStr"/>
+      <c r="J17" s="0" t="inlineStr"/>
+      <c r="K17" s="0" t="inlineStr"/>
+      <c r="L17" s="0" t="inlineStr">
         <is>
           <t>7c5e5730bc8d29fd4a6fb2e9431fcce73b6591a8ace3112d72b35ba7dc3658a9</t>
         </is>
       </c>
-    </row>
-    <row r="18" ht="22" customHeight="1" s="8">
-      <c r="A18" s="2" t="n">
+      <c r="M17" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 9651244833181940040345374803818391185674162523763366310203970155174506339146970261826454534397365565138610929546736658852452675669010441417852005923004326850328952931034021214555469682065237050965109687977216103717131764287685896974426642917859249303914644926181741806886370508333365085737415996230848719288622732241109490318568410982414724576353395578425394512110469973042976997729370215049333240641923962622000125933755550087693065668499393333631768705126138327216839177863099309423025235384880327490403907764444501759693062799623448818291683575594899178179841876692387023751688981877873745560431865320243113936072515648983894502419161374250283716388943938430774785598818355139252323870758322660750279225990789671061773077027532199772220890232751049770677099697193450509325388292458621291582671598055497373652085680695501871545908094431011585963028089811478810529564860438710901500494130752969944441433009884176264122425403829959634331996605382435729057436462764278829099777124244909525792315063819479077950547567782642194917980120127584724779809478943366354238205224790727644786647820608287315096095952790506325586992979359452359200314341167453000743597065334589604014254800342531648097172335095932923717954623809485871301301436631177657392780237729085670317665672395541152902512075794548006266326289975395630491475210452820966749632508467593970351851172490940951716473202744699612368275697090884855889049839855680442455950587024262134980591726425371735803650814386937348499195294099721825689528290138295540633730098746977016074141358461291844149315569988648160386593696380801498248945638526499755928900479250266529710179938924516186062394441442539507037950336982744774961196279447752737952892115602506113504122215168290817593920699584570166500350874335092483948566665496328288578890147610164039789376582991373876618731358304623445932847747724661, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N17" s="0" t="inlineStr"/>
+      <c r="O17" s="0" t="inlineStr"/>
+      <c r="P17" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q17" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R17" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S17" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="22" customHeight="1" s="6">
+      <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="H18" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L18" s="9" t="inlineStr">
+      <c r="B18" s="0" t="inlineStr"/>
+      <c r="C18" s="0" t="inlineStr"/>
+      <c r="D18" s="0" t="inlineStr"/>
+      <c r="E18" s="0" t="inlineStr"/>
+      <c r="F18" s="0" t="inlineStr"/>
+      <c r="G18" s="0" t="inlineStr"/>
+      <c r="H18" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I18" s="0" t="inlineStr"/>
+      <c r="J18" s="0" t="inlineStr"/>
+      <c r="K18" s="0" t="inlineStr"/>
+      <c r="L18" s="0" t="inlineStr">
         <is>
           <t>0ec5d7c7202789681b9c141cbe6d5529e58d0822d5db3508ee16a80833d2979b</t>
         </is>
       </c>
-    </row>
-    <row r="19" ht="22" customHeight="1" s="8">
-      <c r="A19" s="2" t="n">
+      <c r="M18" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 3467675576437412157048909165423610554118050878761144777751237257912773967393704513552811622409415267117093599499169564708689512023417499139906696906699770827910119079722202013085535742153478942033477210111091523025647726048475590902816986581739704661161239874611439247750100561499979382816612924857272669396719572947866224708453000248919449749655669235958146053559964759624626433421162108958371947032266473635396842395402514465252321371051122398687565010009270145723595880945108250813878624933242319462109503647396222320865372971033298228902197244230240483777250622776165988452101282652662171685924637996748160693278276090348492837623904236703169796547249037211295709473628713849004137967590810937822469837892140724980911338658356700076703217959338367581385226278511570949853128185889154078297400219305809844999591578109216868480457763969317635186263953467605584054252218366503839427492304542556842870691833980143078688980200402503246845496052661404174596979879498175484028760351837017858166215739180334681521900194379598155943790301564957450971711401984967539664590199406136302894403396155370596223230928950940931448684249467713946805567543206613963248052194216574002394063727356592349058888547669438115790326334112246910072612159055263649232596682602863043948617388994355857586270070473501937477418419452854842528652566261615603420633496379965475986400335765420128199521904524026791406808505865081163873882112416704903898847355288907654940793851521358901162637418318723833282688908885553233153621137945717735029880246659950687748302267198633378352602850669005224228659643785353593895455128832676974760839390729190659975360856842196187529174240920836407092085408267685336997323652696904500942087601475525121906326992548000015529936193348465649325903034093335959738941736953567243032554990306925011331915890283404265502625878981483138000097760567766, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N18" s="0" t="inlineStr"/>
+      <c r="O18" s="0" t="inlineStr"/>
+      <c r="P18" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q18" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R18" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S18" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="22" customHeight="1" s="6">
+      <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="H19" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L19" s="9" t="inlineStr">
+      <c r="B19" s="0" t="inlineStr"/>
+      <c r="C19" s="0" t="inlineStr"/>
+      <c r="D19" s="0" t="inlineStr"/>
+      <c r="E19" s="0" t="inlineStr"/>
+      <c r="F19" s="0" t="inlineStr"/>
+      <c r="G19" s="0" t="inlineStr"/>
+      <c r="H19" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I19" s="0" t="inlineStr"/>
+      <c r="J19" s="0" t="inlineStr"/>
+      <c r="K19" s="0" t="inlineStr"/>
+      <c r="L19" s="0" t="inlineStr">
         <is>
           <t>90ebd701a32d6e7246e30a26a83f18290f20258895392ef8b608a7a8dd52c16d</t>
         </is>
       </c>
-    </row>
-    <row r="20" ht="22" customHeight="1" s="8">
-      <c r="A20" s="2" t="n">
+      <c r="M19" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 13006256548453269370406199116690988891732730490342308175668679889607024981896603210324925886072541339565405334887475455528806515006795586979143587517502476369345049854373593447073952808430091238464905157338991705232360918805512465126574030898856290316463409412792473806605982493899407032156319492310482756724206282207011848807594767721337645392952131161286773183958798628672578647814067299665572479975567037251143844964598564593819747194930885960179755416019616365328925808247644045848436396220489955684599480037181907430865850260476370779000648218861394992412607197534337592413027690828706584754991541893463317750811663109475413083902192269296982492799989259266101074266673430299565258473429726375033462742821826522574018627212156635654395489565544555499884646621564238272141191393966061956848651508949059740745491041226669442540608612007238492923997649465773168438202304286318869453951137877007500790251317548314090698447022434218910659742357824110732484679433023161126258102723331800041141921411033345939993059191883708291035601339348821923549558264889989547265824885630015937959018740566055744706214664626492625759947068867854660259422204320585777998100886201302850541577089234334269696557412908188387022078499537082409951394559529927413044208201581050171997161942457024575049894293621993960625344924457151219400531455001880152791495331998366501840354211620330512313325460688102482036074012920034027936094003528460885056715977435002048214259967434596804605237496609045777219366635439622358035727922288558985898951870229352381827156156843886280561908564621646235849401365310218665758808734604356984280796828468317686025590943686533939337864283739734313662730596819634959465511796448825063698491775149020573096823451164471332904911061028276281981654651148315101208342495114967772016221971655644902095409549953250612254257027418544188809467195674062, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N19" s="0" t="inlineStr"/>
+      <c r="O19" s="0" t="inlineStr"/>
+      <c r="P19" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q19" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R19" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S19" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="22" customHeight="1" s="6">
+      <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="H20" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L20" s="9" t="inlineStr">
+      <c r="B20" s="0" t="inlineStr"/>
+      <c r="C20" s="0" t="inlineStr"/>
+      <c r="D20" s="0" t="inlineStr"/>
+      <c r="E20" s="0" t="inlineStr"/>
+      <c r="F20" s="0" t="inlineStr"/>
+      <c r="G20" s="0" t="inlineStr"/>
+      <c r="H20" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I20" s="0" t="inlineStr"/>
+      <c r="J20" s="0" t="inlineStr"/>
+      <c r="K20" s="0" t="inlineStr"/>
+      <c r="L20" s="0" t="inlineStr">
         <is>
           <t>d13e378714f99cd1b1f347ab66c4ad14c82aa314a0d5559bea169825a7faed3a</t>
         </is>
       </c>
-    </row>
-    <row r="21" ht="22" customHeight="1" s="8">
-      <c r="A21" s="2" t="n">
+      <c r="M20" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 10128481953109325864503429355442373213937678671696447500287439550674884115753712827754697399440259333281228389441613586687047278272905762264301861962840151189493998031291249943789562449456908312136941247593753164486273685689304285612303312258891156395906616591400693499973650977518078494369047897598547551868637656736634963559916416045921612291028227895572781522989017658707015132407242887833031356191054632541207440587857528879432586835136766275084658805760427106158696558565971448897090714107719042953561558926635555493685354372414482886135366151196111346086573688064923482828900292403859725965896017158598590449088494443425135948053556004142761139939517045754530522640143930655835281244786527821178893304587143036590067999256443524075801196348647260082344893070713917755408928604649777582208060888410440229645810795165591747503737053587745910503435142147246490479076036684360116043760323059294382559531360668018832296551429485298247408037920193765679222122694064077004814401320661207186534153577546123778648095984466686752527461696935075480877622054022674548022605210239719901568763363830002060561989638525401432173663020576602221087971151315455823781032378115025009270988398125050855429597748449049968488395777523429104046976289646474073404238536583008918379438238637732649532599807669164592076809403853821810999037374917238930063771606004635942417204784045718585441606715929625524607687179617112080262794479862103021579005532874232194066250329526930390083720148096287355029409106773689544325989288571705601314287809896724680144097949634395652512838655698043864927220284806010284324534569630479179892754984042950992553479531815266764390530711464509013251801375168309614781703135241332934498251145854779261787885286767307012073260985249631968304384910013899478966208313627303451501327984726293443842857623280319987383163840442672345720848923432136, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N20" s="0" t="inlineStr"/>
+      <c r="O20" s="0" t="inlineStr"/>
+      <c r="P20" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q20" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R20" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S20" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="22" customHeight="1" s="6">
+      <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="H21" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L21" s="9" t="inlineStr">
+      <c r="B21" s="0" t="inlineStr"/>
+      <c r="C21" s="0" t="inlineStr"/>
+      <c r="D21" s="0" t="inlineStr"/>
+      <c r="E21" s="0" t="inlineStr"/>
+      <c r="F21" s="0" t="inlineStr"/>
+      <c r="G21" s="0" t="inlineStr"/>
+      <c r="H21" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I21" s="0" t="inlineStr"/>
+      <c r="J21" s="0" t="inlineStr"/>
+      <c r="K21" s="0" t="inlineStr"/>
+      <c r="L21" s="0" t="inlineStr">
         <is>
           <t>2bdca4a6b122fcc37deb9fc6706b269b1e75a7a4967212f9186318b4e4e88503</t>
         </is>
       </c>
-    </row>
-    <row r="22" ht="22" customHeight="1" s="8">
-      <c r="A22" s="2" t="n">
+      <c r="M21" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 15778462398340306199995056511670159735229005758345764017181700180713154457053399944176855159937032587735506308518744417686242195054022127005103726879021999353555548511442897148444561838015921171839434510896670297080236568581674967102161105253246470714800266735582747421926651744496147728197587098409931225280247527205065488707275765606421007664829036878431413987587332215045810500739453647865486634968746975412947116447826148768995160670141951401129440062023080185020361605052849617522021024734848201545895863225103705671562870055609470174088868906835035650875127443218478107393461901897011223672431500419977936611403620490546289644143846428626653978030160295280065988739302716985016495525708125671999438113296925138735903432120981607621227777478389989269434412071763300360740216580330748194489620152665904294357020998047640098094496824775605198447227618649205736238110679310068520776016080947351684344352950651680644666638552428677865541632060501931254839154156663013148310122991677900900172275361988524904610538242668636493739576326946698634686028490791000585581208196071110666925437259599979332012456154507542377253583571034706807453720455077438628331583292623707333006701444183231986815588668863880117838836202506708281527818664976143162327790469022880220658694469874383911008110668564093812299398723204766077179005286025758934724266975173428727744756152573697837450051659055791649603583291307318463486715931846425679094261203519337892527693666884002857025753039955809632018594529168977788016056129768538087872691817494723327703218997586303744901335854491850078373778767846956528521146965536025491939753939811880451378287581128642648640952761680916450267912591119826973749317160369984067796957328539019544529317989423974493684433612713419733796375803268417189785075508335575526108555431722249802546673797503995647058938685008738251391741843762531, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N21" s="0" t="inlineStr"/>
+      <c r="O21" s="0" t="inlineStr"/>
+      <c r="P21" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q21" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R21" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S21" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="22" customHeight="1" s="6">
+      <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="H22" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L22" s="9" t="inlineStr">
+      <c r="B22" s="0" t="inlineStr"/>
+      <c r="C22" s="0" t="inlineStr"/>
+      <c r="D22" s="0" t="inlineStr"/>
+      <c r="E22" s="0" t="inlineStr"/>
+      <c r="F22" s="0" t="inlineStr"/>
+      <c r="G22" s="0" t="inlineStr"/>
+      <c r="H22" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I22" s="0" t="inlineStr"/>
+      <c r="J22" s="0" t="inlineStr"/>
+      <c r="K22" s="0" t="inlineStr"/>
+      <c r="L22" s="0" t="inlineStr">
         <is>
           <t>f54a7e52f443fbcbca40cfca4da68f4c627ca3984e83bf9ca67e14a142443d7d</t>
         </is>
       </c>
-    </row>
-    <row r="23" ht="22" customHeight="1" s="8">
-      <c r="A23" s="2" t="n">
+      <c r="M22" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 9930472639485816178633022436909132801121969802343846814772465089622973840720325883929498955423183039718823504007683214364995619067565366238605451543677362612328042396474398051056925828010737853604682915534212969588806088754949991780106499123456665010169673242548196798463522748055772585285783031685973007437731907960555346115669992862174340999517301194272147095838634802914945647077536877705690331175295543394159156918546830701098384811617330897884327710848200815310593755939636347414798344648204958055845109872605137442272317700931608272082146473944429091793527042859071048435236357862285421547033684040251102917143414789664256701017072813165326531409283427987651384631618444992548201370648489197096689311941782375759658692656519106355362458541450132256834696990294133054567330822101888320274199854759396508716651215245485697781732266710396627630357690192594598505390452509311767912844201777564519172289957878862782200298259777925289160304331101708525951907665976638713515838464487391070304745139101211703539856456430420859993973766061790159217376295400780139048069543227229150373008499311814094529089801293127759640789783709308317959292029345267679774345112844936918930961962125226603620207236643864903447474674606123490610694133095243363323911433803622781777277238028412535073321845341488673146133168331541421195841378134725923627059445469157231839986838341453429120296010121457331282639711302366540815547192809565862045176834757994962054300823412634360132259144790275397347782495490665164287081553422340465196376138297998172325938317472768362745199353559553793742238588886128322334403664438111609131349306970042062902316914973197113090364935188654377353820344953776148534320192948641749843977357937114798736762841844366485291202396885913057134208879098410102769774361448549570963671714670371935992102408126330917526762568466833201586463576431724, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N22" s="0" t="inlineStr"/>
+      <c r="O22" s="0" t="inlineStr"/>
+      <c r="P22" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q22" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R22" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S22" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="22" customHeight="1" s="6">
+      <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="H23" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L23" s="9" t="inlineStr">
+      <c r="B23" s="0" t="inlineStr"/>
+      <c r="C23" s="0" t="inlineStr"/>
+      <c r="D23" s="0" t="inlineStr"/>
+      <c r="E23" s="0" t="inlineStr"/>
+      <c r="F23" s="0" t="inlineStr"/>
+      <c r="G23" s="0" t="inlineStr"/>
+      <c r="H23" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I23" s="0" t="inlineStr"/>
+      <c r="J23" s="0" t="inlineStr"/>
+      <c r="K23" s="0" t="inlineStr"/>
+      <c r="L23" s="0" t="inlineStr">
         <is>
           <t>7e3e24a8b032247cfc4b28ff038b4c93b8b9bfddadf34195ab96be7eb883aee5</t>
         </is>
       </c>
-    </row>
-    <row r="24" ht="22" customHeight="1" s="8">
-      <c r="A24" s="2" t="n">
+      <c r="M23" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 9823102059526869723940589986945275803449288440292007632754365200279869354581393701289960428572780959671856180311096155168527420759822515451863071901245434873843502816478760828123594227307349614088255284660649335720187434157184180885605527830316580558995333729831104626540883404237029468703655248675015507020401932279433469600659147253005189973853317575643189095616026083467229140589386870784133055070757754189018902647879903226073798742846798195689509286220352633758385217829979058828687699671953668163618814392214759293483882765327217670543442889373944583858988126098338917150919684301274443697994992822665821935269583559279210399334127021790953748331209766412365465842245466977353562355390169740749300487943636835280927062275719058660530086234310727307685716729932297684180636139721956209871185723001047036202151301719714868140696219180670006721954773187981077023244124740340881605042609331245155967808009668992790942579907949166779788218935337456826088643514208577075277999581449220881924046942335898440684964374800359202624945579215934952961059702898410933505524484051858026239051099625575510081340874629618319050500229205845729728256820367504124111661048680189094038611574632439918263664054726457814818714933535518737513760822835521206196298525390660135088475742113203101928157864505744051370515569717428360999601674190871397816157053640951133353219633365704791069740886817098129858827718192547828048301667133517023950576082998933046584291851660384621428748286950867467145096829975376730363276881888417400202304971084682528084493837132620320991116652952492901824429907617230573515443510288724459524882250799218135603510135733922768949754516489395466523418233314538909294467409191223349976585138713292187911804613348290880167083237101948971468080259806730266292345765469402405111513503558009682305103673304459858432777374069150684840690022901316, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N23" s="0" t="inlineStr"/>
+      <c r="O23" s="0" t="inlineStr"/>
+      <c r="P23" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q23" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R23" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S23" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="22" customHeight="1" s="6">
+      <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="H24" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L24" s="9" t="inlineStr">
+      <c r="B24" s="0" t="inlineStr"/>
+      <c r="C24" s="0" t="inlineStr"/>
+      <c r="D24" s="0" t="inlineStr"/>
+      <c r="E24" s="0" t="inlineStr"/>
+      <c r="F24" s="0" t="inlineStr"/>
+      <c r="G24" s="0" t="inlineStr"/>
+      <c r="H24" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I24" s="0" t="inlineStr"/>
+      <c r="J24" s="0" t="inlineStr"/>
+      <c r="K24" s="0" t="inlineStr"/>
+      <c r="L24" s="0" t="inlineStr">
         <is>
           <t>6f5e0a6ca53a7b9c9db778df0e0c1a1b7543a4ea9f8aad71d84546c6657dff59</t>
         </is>
       </c>
-    </row>
-    <row r="25" ht="22" customHeight="1" s="8">
-      <c r="A25" s="2" t="n">
+      <c r="M24" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 15970877267023591790489173612317293414132382861269682591830543792150926285192591555870066313584577562871694061247607611398158670961425706161577462461227918738099621253848857643715389889134634439707015383964026309462889938501955271213161536426622115087524364658557314457648429499298119435624014809772883149219634634233865725413052948405504040354119565024917312630273108729249125181689923882941110249507663026393090401012712458025510146889103421886434046943334950602946588914986755357556002734682414414657876289627348073821501203099666144311893440526546257449816622785946446907441813707337531584153370429055594938087776906183322301784379423435415571873834022163422110511309333064626751473771841619125683116554067642647907766765132673243227459673436080401868247472947966760176915905857351473345169580406792057600147573324056522845831679500108176229613442548023172140796225027164100906097202427299958447000793255363178593121255554206834572808842056550588854327662704341285025952807647677251629471734212614023153014192956846740707063460379087396740456118153621834473206298525741754593430819872670307540478128640324171939852666361426728893745478868383973204624023003665030168288003790854518712851264530556139843156351090560184696129426579289183427520325312939899574882892022044633783659828727113950538391475996197151853302469304446192677941288898442273214149916891197855819602549726773652154103263757791560080468236707311713070248987532120326980051544851993813727875849802904423031990505922146056119421838643360054641101786529368126884083974989709894416528532920650585500989691176555203768069272689152394239243728677156598993556521483091929684793229283064070357818805997010872141682308847029872021644001954174478434324981576238447301910100594119317319217357939717431666045672669540118894453731801450176245482020345941664035143580772360300683409973896840229, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N24" s="0" t="inlineStr"/>
+      <c r="O24" s="0" t="inlineStr"/>
+      <c r="P24" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q24" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R24" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S24" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="22" customHeight="1" s="6">
+      <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="H25" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L25" s="9" t="inlineStr">
+      <c r="B25" s="0" t="inlineStr"/>
+      <c r="C25" s="0" t="inlineStr"/>
+      <c r="D25" s="0" t="inlineStr"/>
+      <c r="E25" s="0" t="inlineStr"/>
+      <c r="F25" s="0" t="inlineStr"/>
+      <c r="G25" s="0" t="inlineStr"/>
+      <c r="H25" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I25" s="0" t="inlineStr"/>
+      <c r="J25" s="0" t="inlineStr"/>
+      <c r="K25" s="0" t="inlineStr"/>
+      <c r="L25" s="0" t="inlineStr">
         <is>
           <t>cc0962acd100498cce9f861bb5b6e3823afe64e81926887e8d592909770d60be</t>
         </is>
       </c>
-    </row>
-    <row r="26" ht="22" customHeight="1" s="8">
-      <c r="A26" s="2" t="n">
+      <c r="M25" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 11163036647868063007681759974619211413070761481818426923663364558638486407475541646450761907563012689802963079834114041606773640400615758506996811260804147330119082260431085855950765409792731479007678236790374173623900495524897036683649987309586907186046742444993766751804109097326493252151961225686419488017115036098974750835545125217014460249328562646642189582578329143720711595121360486554796214170565714177532532954517525779249801424262581158486042658264657014719722731990067598030087141433852026251933228812648928711100710800173756082548630128478224614589349143959351986946684058671352008451733591175135722471827177059378286746101457324810402539332429843698825870806079125725890173987244258514701315970643767734335447549587628029052065505322676637846720940745677060816726532164068717761050349053569684593636562406634927458578665818069093832604922343696976114178102733920776980537574232641737745093656581243840495710959094626444469395443851862273561911141187361876843862389585995656702876733670827253165704720955810016147251047228886339413004394350639465192206475861272328385601246052353919750372268757581801428157540276786480907021367053558587593199216852578236718714261099676771163203641604165562401558250475607837223719365023157012453189677408460815761164407056458338228096127061469256659163257871180993577613588665171879865781314944509684082793116162498801355170268719201865358796429879121071080632808804049720233442990425728531291996598989577471285271088688539807552414370355320205526088106323016686912426883337727424590274337377594509946411675654890912521288986300085653497232988980803320101885398517407083864003014016785433593057250714851843268046967825969172447870439907136424800956776062350250019449343407379592922128702840692253884071612124556121119617388632102247237137939467532073720953075486834464164318787308627528365111677792465170, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N25" s="0" t="inlineStr"/>
+      <c r="O25" s="0" t="inlineStr"/>
+      <c r="P25" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q25" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R25" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S25" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="22" customHeight="1" s="6">
+      <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="H26" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L26" s="9" t="inlineStr">
+      <c r="B26" s="0" t="inlineStr"/>
+      <c r="C26" s="0" t="inlineStr"/>
+      <c r="D26" s="0" t="inlineStr"/>
+      <c r="E26" s="0" t="inlineStr"/>
+      <c r="F26" s="0" t="inlineStr"/>
+      <c r="G26" s="0" t="inlineStr"/>
+      <c r="H26" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I26" s="0" t="inlineStr"/>
+      <c r="J26" s="0" t="inlineStr"/>
+      <c r="K26" s="0" t="inlineStr"/>
+      <c r="L26" s="0" t="inlineStr">
         <is>
           <t>c28b77c43514b557a86a401556134b31c12c7c7fc33ec8319a96301661a70896</t>
         </is>
       </c>
-    </row>
-    <row r="27" ht="22" customHeight="1" s="8">
-      <c r="A27" s="2" t="n">
+      <c r="M26" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 974235465878415798757332680811758270161933765201408330031440103166528831769719979977897377739508574153848739404966816879475016295663243874355605962271021757364053285487020026159654748117653239758952634940686225109546005576881093080192328428719399499701474070592236266150946457902868777685507137759693625086735124280994210038044687031016443832738939819256187782990409000584394725005474382452111483802880185855123669527613821260407526498495832944582098518337684804586375908666633884008454720927342622024388874989167433963139122008160238056905822099106512575467284461625705106170932743964434359113815070647396469521868918059210649453038751732919210221314567572616787976064458032305931523624493791081014782046714908000273886824262481905490715887972325607305274053689945225381210140336980434716566140204990227759492410719341605121953324523356932832896579645590620271951982757680296229346243510987538136577048878219715987495423005683138700315638639796827915113204046970216008602571326688305805461955292165325383527249046945362825944849858547369360855734393031382124264103037661192766482455873031932874478143951186481965924914113328399385256305191998956310619660805591016579026827602705363551781032344721427638250515432536408934219168287162750033953652343137322699346031546260431403302709558668485763676570205339180159647594687470797984735299344765740720782754089605209689499705367785240806734362812450279937097398077313494571774393329018716149095730233855106129425050787871987408487996859248707259430545100433069670217000865262194910924468955217708787737722034136412431903486388862017098452417812810516424798760262279054737862735384095838323271837047032709739894494025174479242138322636386588359592803515390618551820734012731012141875143968121933547567372571161134657867644350936618878787113652530187591898550334204580804868384956827902743546865282032454, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N26" s="0" t="inlineStr"/>
+      <c r="O26" s="0" t="inlineStr"/>
+      <c r="P26" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q26" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R26" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S26" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="22" customHeight="1" s="6">
+      <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="H27" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L27" s="9" t="inlineStr">
+      <c r="B27" s="0" t="inlineStr"/>
+      <c r="C27" s="0" t="inlineStr"/>
+      <c r="D27" s="0" t="inlineStr"/>
+      <c r="E27" s="0" t="inlineStr"/>
+      <c r="F27" s="0" t="inlineStr"/>
+      <c r="G27" s="0" t="inlineStr"/>
+      <c r="H27" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I27" s="0" t="inlineStr"/>
+      <c r="J27" s="0" t="inlineStr"/>
+      <c r="K27" s="0" t="inlineStr"/>
+      <c r="L27" s="0" t="inlineStr">
         <is>
           <t>2fbe5053127216f925da50c84b6040ef929a83cec51edbdfec31700cf011fac9</t>
         </is>
       </c>
-    </row>
-    <row r="28" ht="22" customHeight="1" s="8">
-      <c r="A28" s="2" t="n">
+      <c r="M27" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 9631618087013002072338749395783707683598963050500646478943461571044586821984254343446861840632026545484163279590149630986109846555300459147204236700924206221555436944371841947422746831809371163808692741096358089520730524148758771813882480320884957662641332756987181357364539952979813623228164322925485813709279984288666671515460117538585943117247093824952884821089622887106634341633961821499346430363368189096807554894792148435004607109698123325646902402447657033442583469613476485220043289339958309008367841233733616351936583526531150254253078204809521462996001464806016825858878962294883946834399786450879505030765600126170063162462352283225850280343940962440683240104063939562709615846451856633482045808551526673585124265024666754647933230536596046865603869127861545439275643938065197482164761693409333766649161231727121069966234943430103098237137471048249856253875089595529775209732539470320274183165857536880994470250960520391705992811916663772169990084035006981250747885639037584219839184374175272036557957054751841457049183656840875747360301498809635240202456289079913746321168386822710004183429686100436981256186528349414169128564351004625884986652713315537509640505746611240491727384778563613237979394082348761607063528405598854117156499897597874565557102532689886114936926271833032314815158190174229838144934736873282654225966518993243495945712341549015891279177386424476904953671480639176330333775508840446853325444335003624044089299922218252146217314691143768023500955985819635813030443784105693327945009458322466944380821775509823718201595967976060849180951101831692036483475793194355908085193571650840428952127692513754855234565617686470225800034281928726318588382643343327525732773942961693697831368240275165147588341286466363865073372405513374739054398712551525143730956055927068905055952411172774404298117284261832312119120670677662, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N27" s="0" t="inlineStr"/>
+      <c r="O27" s="0" t="inlineStr"/>
+      <c r="P27" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q27" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R27" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S27" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="22" customHeight="1" s="6">
+      <c r="A28" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="H28" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L28" s="9" t="inlineStr">
+      <c r="B28" s="0" t="inlineStr"/>
+      <c r="C28" s="0" t="inlineStr"/>
+      <c r="D28" s="0" t="inlineStr"/>
+      <c r="E28" s="0" t="inlineStr"/>
+      <c r="F28" s="0" t="inlineStr"/>
+      <c r="G28" s="0" t="inlineStr"/>
+      <c r="H28" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I28" s="0" t="inlineStr"/>
+      <c r="J28" s="0" t="inlineStr"/>
+      <c r="K28" s="0" t="inlineStr"/>
+      <c r="L28" s="0" t="inlineStr">
         <is>
           <t>91d0300c8540b453c538bbdfb3bc5c76a315c1eac46d4f4b655fe5369e6654d3</t>
         </is>
       </c>
-    </row>
-    <row r="29" ht="22" customHeight="1" s="8">
-      <c r="A29" s="2" t="n">
+      <c r="M28" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 6341167419202448333447264932291981084685452014167751182258195108208115537461341029219558833036089411646400502250046478407003883179183978726983164046189720763792578127596753327336122694883286508262094557302659753457777150816316198061716422185500194692763274218234489267442768989087891256194669830913034980099958190866619081605835022124049524232212822284688926798904100518120725946196005809225505101754770694493238174092781676058922047286124424157018650832652934775662256494894233090418273300943233960626683632339255622596372567757893124955138839701141885227110644217239919497273370780587506738057478289173307966856952871661642779691183497686772917602649796452666258286853912502156048249718478213309987642986376411104073760273623150306188856457821188643541739902230500559715122775838062367901043455133917651229505936602561011479553828574903852438449891021021773709237668532729542783562109607470057330273670605462286367802612605935277974407313978188216192838174248522826983685579210401232289878924914871452717155761532172947698868235042838092953733502293638295020563274556818989724354600756381670958995361342795622582982035744975908308347090117843065881487461360221519807614119011597990486191545884876731943953729601994390556503630410433877698014061272186759688632165057649843669625347337691092222309125216100587301936929536758407340406637843756624637696009576075807902727066081363266194490967176959054425850812674685908513810553288625911785207851828435723778296959368244397165071486799668352634782624453514010418437375664073447926073154381755688226608192269006949162826345435721391951399558882355299682134624939480942631820598828928731566846915978103315087716601951300650242315829677262284047600144512593172547711046378648971137204223030047320904225849971302476392963923657953802264049139638351294302960279222356294787869524877541014169957674856470955, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N28" s="0" t="inlineStr"/>
+      <c r="O28" s="0" t="inlineStr"/>
+      <c r="P28" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q28" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R28" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S28" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="22" customHeight="1" s="6">
+      <c r="A29" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="H29" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L29" s="9" t="inlineStr">
+      <c r="B29" s="0" t="inlineStr"/>
+      <c r="C29" s="0" t="inlineStr"/>
+      <c r="D29" s="0" t="inlineStr"/>
+      <c r="E29" s="0" t="inlineStr"/>
+      <c r="F29" s="0" t="inlineStr"/>
+      <c r="G29" s="0" t="inlineStr"/>
+      <c r="H29" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I29" s="0" t="inlineStr"/>
+      <c r="J29" s="0" t="inlineStr"/>
+      <c r="K29" s="0" t="inlineStr"/>
+      <c r="L29" s="0" t="inlineStr">
         <is>
           <t>652c4820522764f9a5f59846fa519b1a8c1295bff73070c22c891dfa6f3152c3</t>
         </is>
       </c>
-    </row>
-    <row r="30" ht="22" customHeight="1" s="8">
-      <c r="A30" s="2" t="n">
+      <c r="M29" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 16667666350003629224742184091403532648549990655206509130262235559144011253744049367766030822260684545048855126532923466486553360933551943899965527233342533230224482056891607865266458790476296944933617987562580966878271058724198311870779400079194351108788995684147365210156912441704966783897340952251486736161291313724156254052218127936531138668661034001666238006461391959346772864726027529095188725494426183042430790188756226088427386184888789631593429466033463522248790459715784139383851638838844068557204418239373253095075114366840170297349450254882233490213664931437127737834196007061519490305980957685465125735081476018819785247879022590228297896908893775508324245198627685567492237360385941955661230180497378874871601195113594738867778932517443839690979869831143669602051289190781035636735413707070516727699401695673540814903051347032864130711644410263354964450083826135425697425344260630557780669790401901212417270337820374416009112502309849546178612474157584136490320359334306833523649453878985392073943041827440219106520844408578577308342186724556060330710712092352580687394161400350745016222166003301146978708814670621953568375855695321341650366785583784877739950053474539530361525848395868583759545143576363464236469442298426612979829046574161308514762953703719734438455440477739815202771657271679226024632068613093400659605271079063087108524577748621251172074895402351003636763389670701871511689792061117325077519379759857278507365862086953457526128201946484005987891608670541909365972515845374968998981617515688219903606058141782483503406396093654380886959866753577028311153842239585725892962191590136115710149148602259729380359054292468546734637606940299110994838289298018662266359020278713321973248384005425158806334252441565470036885113923718843302247820629288641231551193237874863201089201224355260310030485187281805753668900550295982, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N29" s="0" t="inlineStr"/>
+      <c r="O29" s="0" t="inlineStr"/>
+      <c r="P29" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q29" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R29" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S29" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="22" customHeight="1" s="6">
+      <c r="A30" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="H30" s="10" t="n">
-        <v>10000</v>
-      </c>
-      <c r="L30" s="9" t="inlineStr">
+      <c r="B30" s="0" t="inlineStr"/>
+      <c r="C30" s="0" t="inlineStr"/>
+      <c r="D30" s="0" t="inlineStr"/>
+      <c r="E30" s="0" t="inlineStr"/>
+      <c r="F30" s="0" t="inlineStr"/>
+      <c r="G30" s="0" t="inlineStr"/>
+      <c r="H30" s="13" t="n">
+        <v>10000</v>
+      </c>
+      <c r="I30" s="0" t="inlineStr"/>
+      <c r="J30" s="0" t="inlineStr"/>
+      <c r="K30" s="0" t="inlineStr"/>
+      <c r="L30" s="0" t="inlineStr">
         <is>
           <t>8fbc2da00cb3831d1527925fb4d272e4135b36bb1b604d3ee58266c9d3ea43df</t>
+        </is>
+      </c>
+      <c r="M30" s="0" t="inlineStr">
+        <is>
+          <t>[{"ciphertext": 14632789407775493606236852920988207291352288344931401008296755212289929573744348065782875917914743825816999491923993801421554397529122423618887351570734684227644221552004207159467228083977923826900740220470871256604943796598847416849988606035433942599683024564323572709978136875518237372611047563088440726337756671670654244583061053380886101350442447385980008196961530337085275417842799773631204752682270631810186049536665301728066275761463812263503753572371713494503583941409877753419901951466020812172907991150131478385656331711532122946003439711074001246467688148348803070824042586125476607494192069728993542037878950686697756499715931588003308766729215270058227933517081222838052042344218032377275331872993940326262980306478152027087096678007567488027568133043182857528016207558388291635390322966362914799115233030326506992283357066803451859002782338034208393893000971336226780111136673221897467009977944157540226185944927184945063111326676511606773804545677207031840732509345649890196640149649951925545742405943167368820032251400461467890499498621248858426722901263872771693588372995693410765694398062061100753941984304207123434338553024798993806524807934921422333403552299134574384697308928164117086929534093520848730962163233813520209298875404096056682459374354579094269677545568901620150805035790957970389002395671608002312161508149727398638633338116304056135357671461432252453950443240928402724591985513394995577205169002088489294052450830622067019189713596355066556055449570703220460250981595023361189989490448832896876834226598273190305962885069203978007422525504916574255872497852116662619857293424047977793876178513401144706423881017701537334574470960750778039937165621669952918921285173205528782823157993267169150600734844657931317048345092060832271788901055271271054527685227269352555126511084564088276326737693502773117107370489620237, "exponent": 0}]</t>
+        </is>
+      </c>
+      <c r="N30" s="0" t="inlineStr"/>
+      <c r="O30" s="0" t="inlineStr"/>
+      <c r="P30" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x1176d6f10&gt;</t>
+        </is>
+      </c>
+      <c r="Q30" s="0" t="inlineStr">
+        <is>
+          <t>&lt;phe.paillier.EncryptedNumber object at 0x117a83640&gt;</t>
+        </is>
+      </c>
+      <c r="R30" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
+        </is>
+      </c>
+      <c r="S30" s="0" t="inlineStr">
+        <is>
+          <t>f74907b790861eaca4e2b401c67a7798bbe67d8cd76379e99063e7afc4a5ecf3</t>
         </is>
       </c>
     </row>
@@ -1034,164 +2139,164 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col width="7.83203125" customWidth="1" style="8" min="1" max="1"/>
-    <col width="24.1640625" customWidth="1" style="8" min="2" max="2"/>
-    <col width="44.5" customWidth="1" style="8" min="3" max="3"/>
-    <col width="24.6640625" customWidth="1" style="8" min="4" max="4"/>
-    <col width="24.1640625" customWidth="1" style="8" min="5" max="5"/>
-    <col width="29.6640625" customWidth="1" style="8" min="6" max="6"/>
-    <col width="30.83203125" customWidth="1" style="8" min="7" max="7"/>
-    <col width="31.5" customWidth="1" style="8" min="8" max="8"/>
-    <col width="31.33203125" customWidth="1" style="8" min="9" max="9"/>
+    <col width="7.83203125" customWidth="1" style="6" min="1" max="1"/>
+    <col width="24.1640625" customWidth="1" style="6" min="2" max="2"/>
+    <col width="44.5" customWidth="1" style="6" min="3" max="3"/>
+    <col width="24.6640625" customWidth="1" style="6" min="4" max="4"/>
+    <col width="24.1640625" customWidth="1" style="6" min="5" max="5"/>
+    <col width="29.6640625" customWidth="1" style="6" min="6" max="6"/>
+    <col width="30.83203125" customWidth="1" style="6" min="7" max="7"/>
+    <col width="31.5" customWidth="1" style="6" min="8" max="8"/>
+    <col width="31.33203125" customWidth="1" style="6" min="9" max="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="32" customHeight="1" s="8">
-      <c r="A1" s="5" t="inlineStr">
+    <row r="1" ht="32" customHeight="1" s="6">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>#</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>hashed-AT-info</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>2-sig-receipt-verification-refercence</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>DEA-debit</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>DEA-credit</t>
         </is>
       </c>
-      <c r="F1" s="5" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>HE_pk_sender(amount)</t>
         </is>
       </c>
-      <c r="G1" s="5" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>HE_pk_recipient(amount)</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="22" customHeight="1" s="8">
-      <c r="A2" s="6" t="n">
+    <row r="2" ht="22" customHeight="1" s="6">
+      <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="22" customHeight="1" s="8">
-      <c r="A3" s="6" t="n">
+    <row r="3" ht="22" customHeight="1" s="6">
+      <c r="A3" s="4" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="4" ht="22" customHeight="1" s="8">
-      <c r="A4" s="6" t="n">
+    <row r="4" ht="22" customHeight="1" s="6">
+      <c r="A4" s="4" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="5" ht="22" customHeight="1" s="8">
-      <c r="A5" s="6" t="n">
+    <row r="5" ht="22" customHeight="1" s="6">
+      <c r="A5" s="4" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="6" ht="22" customHeight="1" s="8">
-      <c r="A6" s="6" t="n">
+    <row r="6" ht="22" customHeight="1" s="6">
+      <c r="A6" s="4" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="7" ht="22" customHeight="1" s="8">
-      <c r="A7" s="6" t="n">
+    <row r="7" ht="22" customHeight="1" s="6">
+      <c r="A7" s="4" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="8" ht="22" customHeight="1" s="8">
-      <c r="A8" s="6" t="n">
+    <row r="8" ht="22" customHeight="1" s="6">
+      <c r="A8" s="4" t="n">
         <v>7</v>
       </c>
     </row>
-    <row r="9" ht="22" customHeight="1" s="8">
-      <c r="A9" s="6" t="n">
+    <row r="9" ht="22" customHeight="1" s="6">
+      <c r="A9" s="4" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="10" ht="22" customHeight="1" s="8">
-      <c r="A10" s="6" t="n">
+    <row r="10" ht="22" customHeight="1" s="6">
+      <c r="A10" s="4" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="11" ht="22" customHeight="1" s="8">
-      <c r="A11" s="6" t="n">
+    <row r="11" ht="22" customHeight="1" s="6">
+      <c r="A11" s="4" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="12" ht="22" customHeight="1" s="8">
-      <c r="A12" s="6" t="n">
+    <row r="12" ht="22" customHeight="1" s="6">
+      <c r="A12" s="4" t="n">
         <v>11</v>
       </c>
     </row>
-    <row r="13" ht="22" customHeight="1" s="8">
-      <c r="A13" s="6" t="n">
+    <row r="13" ht="22" customHeight="1" s="6">
+      <c r="A13" s="4" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="14" ht="22" customHeight="1" s="8">
-      <c r="A14" s="6" t="n">
+    <row r="14" ht="22" customHeight="1" s="6">
+      <c r="A14" s="4" t="n">
         <v>13</v>
       </c>
     </row>
-    <row r="15" ht="22" customHeight="1" s="8">
-      <c r="A15" s="6" t="n">
+    <row r="15" ht="22" customHeight="1" s="6">
+      <c r="A15" s="4" t="n">
         <v>14</v>
       </c>
     </row>
-    <row r="16" ht="22" customHeight="1" s="8">
-      <c r="A16" s="6" t="n">
+    <row r="16" ht="22" customHeight="1" s="6">
+      <c r="A16" s="4" t="n">
         <v>15</v>
       </c>
     </row>
-    <row r="17" ht="22" customHeight="1" s="8">
-      <c r="A17" s="6" t="n">
+    <row r="17" ht="22" customHeight="1" s="6">
+      <c r="A17" s="4" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="18" ht="22" customHeight="1" s="8">
-      <c r="A18" s="6" t="n">
+    <row r="18" ht="22" customHeight="1" s="6">
+      <c r="A18" s="4" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="19" ht="22" customHeight="1" s="8">
-      <c r="A19" s="6" t="n">
+    <row r="19" ht="22" customHeight="1" s="6">
+      <c r="A19" s="4" t="n">
         <v>18</v>
       </c>
     </row>
-    <row r="20" ht="22" customHeight="1" s="8">
-      <c r="A20" s="6" t="n">
+    <row r="20" ht="22" customHeight="1" s="6">
+      <c r="A20" s="4" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="21" ht="22" customHeight="1" s="8">
-      <c r="A21" s="6" t="n">
+    <row r="21" ht="22" customHeight="1" s="6">
+      <c r="A21" s="4" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="22" ht="22" customHeight="1" s="8">
-      <c r="A22" s="6" t="n">
+    <row r="22" ht="22" customHeight="1" s="6">
+      <c r="A22" s="4" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="7" t="n"/>
+      <c r="A23" s="5" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="7" t="n"/>
+      <c r="A24" s="5" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>